<commit_message>
updated figure 5 to use best rmse in Excel and PPT; added results section in report
</commit_message>
<xml_diff>
--- a/plots.xlsx
+++ b/plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fig3" sheetId="1" r:id="rId1"/>
@@ -332,11 +332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104199216"/>
-        <c:axId val="-2096939616"/>
+        <c:axId val="-2094002528"/>
+        <c:axId val="-2093983984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104199216"/>
+        <c:axId val="-2094002528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -442,13 +442,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096939616"/>
+        <c:crossAx val="-2093983984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2096939616"/>
+        <c:axId val="-2093983984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.1"/>
@@ -564,7 +564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2104199216"/>
+        <c:crossAx val="-2094002528"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1918,11 +1918,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2086033424"/>
-        <c:axId val="-2082140000"/>
+        <c:axId val="-2089597376"/>
+        <c:axId val="-2089592272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2086033424"/>
+        <c:axId val="-2089597376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.7"/>
@@ -2032,12 +2032,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082140000"/>
+        <c:crossAx val="-2089592272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2082140000"/>
+        <c:axId val="-2089592272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -2146,7 +2146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086033424"/>
+        <c:crossAx val="-2089597376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2544,19 +2544,19 @@
                   <c:v>0.0978717157408745</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.104636128768716</c:v>
+                  <c:v>0.102232230021545</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.113223119581849</c:v>
+                  <c:v>0.107911538549888</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.133848921663863</c:v>
+                  <c:v>0.118970856835494</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.170296248688942</c:v>
+                  <c:v>0.138213421952985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.306112485114078</c:v>
+                  <c:v>0.182122541185623</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2571,11 +2571,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2081868512"/>
-        <c:axId val="-2075103904"/>
+        <c:axId val="-2061647088"/>
+        <c:axId val="2145322416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2081868512"/>
+        <c:axId val="-2061647088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2684,14 +2684,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2075103904"/>
+        <c:crossAx val="2145322416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2075103904"/>
+        <c:axId val="2145322416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.08"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2797,7 +2798,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081868512"/>
+        <c:crossAx val="-2061647088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4884,7 +4885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -4965,7 +4966,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection sqref="A1:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5218,8 +5219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5285,7 +5286,7 @@
         <v>0.6</v>
       </c>
       <c r="B8">
-        <v>0.104636128768716</v>
+        <v>0.102232230021545</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -5293,7 +5294,7 @@
         <v>0.7</v>
       </c>
       <c r="B9">
-        <v>0.113223119581849</v>
+        <v>0.107911538549888</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -5301,7 +5302,7 @@
         <v>0.8</v>
       </c>
       <c r="B10">
-        <v>0.133848921663863</v>
+        <v>0.11897085683549399</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -5309,7 +5310,7 @@
         <v>0.9</v>
       </c>
       <c r="B11">
-        <v>0.170296248688942</v>
+        <v>0.138213421952985</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5317,7 +5318,7 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>0.30611248511407801</v>
+        <v>0.18212254118562299</v>
       </c>
     </row>
   </sheetData>
@@ -5328,10 +5329,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B15" sqref="B15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5868,6 +5869,52 @@
         <v>2.2883067854547701</v>
       </c>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f>MIN(B2:B14)</f>
+        <v>9.1333492631906404E-2</v>
+      </c>
+      <c r="C15">
+        <f>MIN(C2:C14)</f>
+        <v>9.0276306442998402E-2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:L15" si="0">MIN(D2:D14)</f>
+        <v>9.0263265154279099E-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>9.1316370758817406E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>9.3660764824055803E-2</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>9.7871715740874499E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.102232230021545</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.107911538549888</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.11897085683549399</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>0.138213421952985</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0.18212254118562299</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>